<commit_message>
Mẫu 39, Tạo các Form Creat Doc
</commit_message>
<xml_diff>
--- a/123-2022-CUVT-ANSV-DTRR-KHMS/PO1/DP1666-2022/Mẫu 27. Biên bản bàn giao HH kho ANSV_KTM.xlsx
+++ b/123-2022-CUVT-ANSV-DTRR-KHMS/PO1/DP1666-2022/Mẫu 27. Biên bản bàn giao HH kho ANSV_KTM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OPM\123-2022-CUVT-ANSV-DTRR-KHMS\PO1\DP1666-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8626DAF1-820D-4481-9ED2-CE0592939A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D6CB5F3-3445-423D-9769-7806C630FE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="1740" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2420" yWindow="2420" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mẫu giao hàng" sheetId="6" r:id="rId1"/>

</xml_diff>